<commit_message>
messing the data up more
</commit_message>
<xml_diff>
--- a/week1/experimental_data.xlsx
+++ b/week1/experimental_data.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10908"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/khertwec/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{541099D7-C915-0845-B676-BFDD483F32BB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8199308F-1D2E-5F4F-806B-CBF8E11C11B2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11360" yWindow="2900" windowWidth="25120" windowHeight="15580" tabRatio="481"/>
+    <workbookView xWindow="14220" yWindow="5220" windowWidth="25120" windowHeight="15580" tabRatio="481" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2013" sheetId="1" r:id="rId1"/>
     <sheet name="2014" sheetId="2" r:id="rId2"/>
-    <sheet name="dates" sheetId="6" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
@@ -30,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="43">
   <si>
     <t>M</t>
   </si>
@@ -50,12 +49,6 @@
     <t>Date collected</t>
   </si>
   <si>
-    <t>Species</t>
-  </si>
-  <si>
-    <t>Plot: 3</t>
-  </si>
-  <si>
     <t>33g</t>
   </si>
   <si>
@@ -156,16 +149,25 @@
   </si>
   <si>
     <t>Experiment</t>
+  </si>
+  <si>
+    <t>Weight (g)</t>
+  </si>
+  <si>
+    <t>M*</t>
+  </si>
+  <si>
+    <t>Weight (grams)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="m/d;@"/>
+    <numFmt numFmtId="164" formatCode="m/d;@"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -192,10 +194,6 @@
     <font>
       <b/>
       <sz val="24"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <sz val="16"/>
       <name val="Arial"/>
     </font>
     <font>
@@ -337,7 +335,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -345,11 +343,10 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
@@ -361,8 +358,6 @@
     <xf numFmtId="14" fontId="4" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -754,7 +749,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43e0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:effectLst>
                 <a:outerShdw blurRad="63500" dist="38099" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="000000">
@@ -798,7 +793,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43e0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:effectLst>
                 <a:outerShdw blurRad="63500" dist="38099" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="000000">
@@ -819,11 +814,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="C3:X28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
-      <selection activeCell="I26" sqref="I26"/>
+    <sheetView zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
+      <selection activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="25" x14ac:dyDescent="0.25"/>
@@ -845,8 +840,8 @@
   </cols>
   <sheetData>
     <row r="3" spans="3:13" ht="79" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C3" s="12" t="s">
-        <v>25</v>
+      <c r="C3" s="11" t="s">
+        <v>23</v>
       </c>
       <c r="D3" s="5"/>
       <c r="E3" s="5"/>
@@ -886,376 +881,376 @@
       <c r="M5" s="5"/>
     </row>
     <row r="6" spans="3:13" ht="30" x14ac:dyDescent="0.3">
-      <c r="C6" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="D6" s="14"/>
-      <c r="E6" s="14"/>
-      <c r="F6" s="15"/>
+      <c r="C6" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="D6" s="13"/>
+      <c r="E6" s="13"/>
+      <c r="F6" s="14"/>
       <c r="G6" s="5"/>
       <c r="H6" s="5"/>
-      <c r="I6" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="J6" s="14"/>
-      <c r="K6" s="14"/>
-      <c r="L6" s="15"/>
+      <c r="I6" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="J6" s="13"/>
+      <c r="K6" s="13"/>
+      <c r="L6" s="14"/>
       <c r="M6" s="5"/>
     </row>
     <row r="7" spans="3:13" ht="30" x14ac:dyDescent="0.3">
-      <c r="C7" s="16" t="s">
+      <c r="C7" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="D7" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="E7" s="17" t="s">
+      <c r="D7" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="E7" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="F7" s="18" t="s">
+      <c r="F7" s="17" t="s">
         <v>4</v>
       </c>
       <c r="G7" s="5"/>
       <c r="H7" s="5"/>
-      <c r="I7" s="16" t="s">
+      <c r="I7" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="J7" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="K7" s="17" t="s">
+      <c r="J7" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="K7" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="L7" s="18" t="s">
-        <v>4</v>
+      <c r="L7" s="17" t="s">
+        <v>40</v>
       </c>
       <c r="M7" s="5"/>
     </row>
     <row r="8" spans="3:13" ht="30" x14ac:dyDescent="0.3">
-      <c r="C8" s="19">
+      <c r="C8" s="18">
         <v>41471</v>
       </c>
-      <c r="D8" s="17">
-        <v>1</v>
-      </c>
-      <c r="E8" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="F8" s="18"/>
+      <c r="D8" s="16">
+        <v>1</v>
+      </c>
+      <c r="E8" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="F8" s="17"/>
       <c r="G8" s="5"/>
       <c r="H8" s="5"/>
-      <c r="I8" s="19">
+      <c r="I8" s="18">
         <v>41590</v>
       </c>
-      <c r="J8" s="17">
+      <c r="J8" s="16">
         <v>4</v>
       </c>
-      <c r="K8" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="L8" s="18">
+      <c r="K8" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="L8" s="17">
         <v>117</v>
       </c>
       <c r="M8" s="5"/>
     </row>
     <row r="9" spans="3:13" ht="30" x14ac:dyDescent="0.3">
-      <c r="C9" s="19">
+      <c r="C9" s="18">
         <v>41471</v>
       </c>
-      <c r="D9" s="17">
+      <c r="D9" s="16">
         <v>2</v>
       </c>
-      <c r="E9" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="F9" s="18" t="s">
-        <v>8</v>
+      <c r="E9" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="F9" s="17" t="s">
+        <v>6</v>
       </c>
       <c r="G9" s="5"/>
       <c r="H9" s="5"/>
-      <c r="I9" s="19">
+      <c r="I9" s="18">
         <v>41590</v>
       </c>
-      <c r="J9" s="17">
+      <c r="J9" s="16">
         <v>3</v>
       </c>
-      <c r="K9" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="L9" s="18">
+      <c r="K9" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="L9" s="17">
         <v>121</v>
       </c>
       <c r="M9" s="5"/>
     </row>
     <row r="10" spans="3:13" ht="30" x14ac:dyDescent="0.3">
-      <c r="C10" s="19">
+      <c r="C10" s="18">
         <v>41471</v>
       </c>
-      <c r="D10" s="17">
+      <c r="D10" s="16">
         <v>4</v>
       </c>
-      <c r="E10" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="F10" s="18"/>
+      <c r="E10" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="F10" s="17"/>
       <c r="G10" s="5"/>
       <c r="H10" s="5"/>
-      <c r="I10" s="19">
+      <c r="I10" s="18">
         <v>41590</v>
       </c>
-      <c r="J10" s="17">
+      <c r="J10" s="16">
         <v>2</v>
       </c>
-      <c r="K10" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="L10" s="18">
+      <c r="K10" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="L10" s="17">
         <v>115</v>
       </c>
       <c r="M10" s="5"/>
     </row>
     <row r="11" spans="3:13" ht="30" x14ac:dyDescent="0.3">
-      <c r="C11" s="19">
+      <c r="C11" s="18">
         <v>41471</v>
       </c>
-      <c r="D11" s="17">
+      <c r="D11" s="16">
         <v>3</v>
       </c>
-      <c r="E11" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="F11" s="18"/>
+      <c r="E11" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="F11" s="17"/>
       <c r="G11" s="5"/>
       <c r="H11" s="5"/>
-      <c r="I11" s="19">
+      <c r="I11" s="18">
         <v>41590</v>
       </c>
-      <c r="J11" s="17">
-        <v>1</v>
-      </c>
-      <c r="K11" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="L11" s="18">
+      <c r="J11" s="16">
+        <v>1</v>
+      </c>
+      <c r="K11" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="L11" s="17">
         <v>120</v>
       </c>
       <c r="M11" s="5"/>
     </row>
     <row r="12" spans="3:13" ht="30" x14ac:dyDescent="0.3">
-      <c r="C12" s="19">
+      <c r="C12" s="18">
         <v>41473</v>
       </c>
-      <c r="D12" s="17">
+      <c r="D12" s="16">
         <v>4</v>
       </c>
-      <c r="E12" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="F12" s="18" t="s">
-        <v>9</v>
+      <c r="E12" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="F12" s="17" t="s">
+        <v>7</v>
       </c>
       <c r="G12" s="5"/>
       <c r="H12" s="5"/>
-      <c r="I12" s="19">
+      <c r="I12" s="18">
         <v>41591</v>
       </c>
-      <c r="J12" s="17">
+      <c r="J12" s="16">
         <v>3</v>
       </c>
-      <c r="K12" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="L12" s="18">
+      <c r="K12" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="L12" s="17">
         <v>118</v>
       </c>
       <c r="M12" s="5"/>
     </row>
     <row r="13" spans="3:13" ht="30" x14ac:dyDescent="0.3">
-      <c r="C13" s="19">
+      <c r="C13" s="18">
         <v>41473</v>
       </c>
-      <c r="D13" s="17">
+      <c r="D13" s="16">
         <v>2</v>
       </c>
-      <c r="E13" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="F13" s="18" t="s">
-        <v>10</v>
+      <c r="E13" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="F13" s="17" t="s">
+        <v>8</v>
       </c>
       <c r="G13" s="5"/>
       <c r="H13" s="5"/>
-      <c r="I13" s="19">
+      <c r="I13" s="18">
         <v>41591</v>
       </c>
-      <c r="J13" s="17">
+      <c r="J13" s="16">
         <v>2</v>
       </c>
-      <c r="K13" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="L13" s="18">
+      <c r="K13" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="L13" s="17">
         <v>126</v>
       </c>
       <c r="M13" s="5"/>
     </row>
     <row r="14" spans="3:13" ht="30" x14ac:dyDescent="0.3">
-      <c r="C14" s="19">
+      <c r="C14" s="18">
         <v>41473</v>
       </c>
-      <c r="D14" s="17">
+      <c r="D14" s="16">
         <v>4</v>
       </c>
-      <c r="E14" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="F14" s="18" t="s">
-        <v>11</v>
+      <c r="E14" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="F14" s="17" t="s">
+        <v>9</v>
       </c>
       <c r="G14" s="5"/>
       <c r="H14" s="5"/>
-      <c r="I14" s="19">
+      <c r="I14" s="18">
         <v>41591</v>
       </c>
-      <c r="J14" s="17">
-        <v>1</v>
-      </c>
-      <c r="K14" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="L14" s="18" t="s">
-        <v>19</v>
+      <c r="J14" s="16">
+        <v>1</v>
+      </c>
+      <c r="K14" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="L14" s="17" t="s">
+        <v>17</v>
       </c>
       <c r="M14" s="5"/>
     </row>
     <row r="15" spans="3:13" ht="30" x14ac:dyDescent="0.3">
-      <c r="C15" s="19">
+      <c r="C15" s="18">
         <v>41473</v>
       </c>
-      <c r="D15" s="17">
+      <c r="D15" s="16">
         <v>3</v>
       </c>
-      <c r="E15" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="F15" s="18" t="s">
-        <v>12</v>
+      <c r="E15" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="F15" s="17" t="s">
+        <v>10</v>
       </c>
       <c r="G15" s="5"/>
       <c r="H15" s="5"/>
-      <c r="I15" s="19">
+      <c r="I15" s="18">
         <v>41591</v>
       </c>
-      <c r="J15" s="17">
+      <c r="J15" s="16">
         <v>2</v>
       </c>
-      <c r="K15" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="L15" s="18" t="s">
-        <v>20</v>
+      <c r="K15" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="L15" s="17" t="s">
+        <v>18</v>
       </c>
       <c r="M15" s="5"/>
     </row>
     <row r="16" spans="3:13" ht="30" x14ac:dyDescent="0.3">
-      <c r="C16" s="19">
+      <c r="C16" s="18">
         <v>41473</v>
       </c>
-      <c r="D16" s="17">
+      <c r="D16" s="16">
         <v>2</v>
       </c>
-      <c r="E16" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="F16" s="18" t="s">
-        <v>13</v>
+      <c r="E16" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="F16" s="17" t="s">
+        <v>11</v>
       </c>
       <c r="G16" s="5"/>
       <c r="H16" s="5"/>
-      <c r="I16" s="19">
+      <c r="I16" s="18">
         <v>41591</v>
       </c>
-      <c r="J16" s="17">
+      <c r="J16" s="16">
         <v>2</v>
       </c>
-      <c r="K16" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="L16" s="18">
+      <c r="K16" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="L16" s="17">
         <v>122</v>
       </c>
       <c r="M16" s="5"/>
     </row>
     <row r="17" spans="3:13" ht="30" x14ac:dyDescent="0.3">
-      <c r="C17" s="19">
+      <c r="C17" s="18">
         <v>41473</v>
       </c>
-      <c r="D17" s="17">
-        <v>1</v>
-      </c>
-      <c r="E17" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="F17" s="18" t="s">
-        <v>14</v>
+      <c r="D17" s="16">
+        <v>1</v>
+      </c>
+      <c r="E17" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="F17" s="17" t="s">
+        <v>12</v>
       </c>
       <c r="G17" s="5"/>
       <c r="H17" s="5"/>
-      <c r="I17" s="19">
+      <c r="I17" s="18">
         <v>41591</v>
       </c>
-      <c r="J17" s="17">
+      <c r="J17" s="16">
         <v>3</v>
       </c>
-      <c r="K17" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="L17" s="18">
+      <c r="K17" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="L17" s="17">
         <v>107</v>
       </c>
       <c r="M17" s="5"/>
     </row>
     <row r="18" spans="3:13" ht="30" x14ac:dyDescent="0.3">
-      <c r="C18" s="19">
+      <c r="C18" s="18">
         <v>41473</v>
       </c>
-      <c r="D18" s="17">
+      <c r="D18" s="16">
         <v>2</v>
       </c>
-      <c r="E18" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="F18" s="18" t="s">
-        <v>15</v>
+      <c r="E18" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="F18" s="17" t="s">
+        <v>13</v>
       </c>
       <c r="G18" s="5"/>
       <c r="H18" s="5"/>
-      <c r="I18" s="20">
+      <c r="I18" s="19">
         <v>41591</v>
       </c>
-      <c r="J18" s="21">
+      <c r="J18" s="20">
         <v>4</v>
       </c>
-      <c r="K18" s="21" t="s">
-        <v>1</v>
-      </c>
-      <c r="L18" s="22">
+      <c r="K18" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="L18" s="21">
         <v>115</v>
       </c>
       <c r="M18" s="5"/>
     </row>
     <row r="19" spans="3:13" ht="30" x14ac:dyDescent="0.3">
-      <c r="C19" s="19">
+      <c r="C19" s="18">
         <v>41473</v>
       </c>
-      <c r="D19" s="17">
+      <c r="D19" s="16">
         <v>3</v>
       </c>
-      <c r="E19" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="F19" s="18" t="s">
-        <v>16</v>
+      <c r="E19" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="F19" s="17" t="s">
+        <v>14</v>
       </c>
       <c r="G19" s="5"/>
       <c r="H19" s="5"/>
@@ -1266,17 +1261,17 @@
       <c r="M19" s="5"/>
     </row>
     <row r="20" spans="3:13" ht="30" x14ac:dyDescent="0.3">
-      <c r="C20" s="19">
+      <c r="C20" s="18">
         <v>41473</v>
       </c>
-      <c r="D20" s="17">
+      <c r="D20" s="16">
         <v>4</v>
       </c>
-      <c r="E20" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="F20" s="18" t="s">
-        <v>17</v>
+      <c r="E20" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="F20" s="17" t="s">
+        <v>15</v>
       </c>
       <c r="G20" s="5"/>
       <c r="H20" s="5"/>
@@ -1287,17 +1282,17 @@
       <c r="M20" s="5"/>
     </row>
     <row r="21" spans="3:13" ht="30" x14ac:dyDescent="0.3">
-      <c r="C21" s="20">
+      <c r="C21" s="19">
         <v>41473</v>
       </c>
-      <c r="D21" s="21">
+      <c r="D21" s="20">
         <v>3</v>
       </c>
-      <c r="E21" s="21" t="s">
-        <v>1</v>
-      </c>
-      <c r="F21" s="22" t="s">
-        <v>18</v>
+      <c r="E21" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="F21" s="21" t="s">
+        <v>16</v>
       </c>
       <c r="G21" s="5"/>
       <c r="H21" s="5"/>
@@ -1410,11 +1405,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="C2:S47"/>
   <sheetViews>
-    <sheetView zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView tabSelected="1" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
+      <selection activeCell="P8" sqref="P8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="25" x14ac:dyDescent="0.25"/>
@@ -1432,26 +1427,26 @@
   <sheetData>
     <row r="2" spans="3:17" ht="69" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C2" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="3:17" ht="30" x14ac:dyDescent="0.3">
       <c r="C6" s="4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
       <c r="G6" s="5"/>
       <c r="H6" s="4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="I6" s="4"/>
       <c r="J6" s="4"/>
       <c r="K6" s="4"/>
       <c r="L6" s="5"/>
       <c r="M6" s="4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="N6" s="4"/>
       <c r="O6" s="4"/>
@@ -1463,7 +1458,7 @@
         <v>5</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E7" s="4" t="s">
         <v>3</v>
@@ -1476,7 +1471,7 @@
         <v>5</v>
       </c>
       <c r="I7" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="J7" s="4" t="s">
         <v>3</v>
@@ -1489,13 +1484,13 @@
         <v>5</v>
       </c>
       <c r="N7" s="4" t="s">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="O7" s="4" t="s">
         <v>3</v>
       </c>
       <c r="P7" s="4" t="s">
-        <v>4</v>
+        <v>42</v>
       </c>
       <c r="Q7" s="5"/>
     </row>
@@ -1504,7 +1499,7 @@
         <v>41648</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E8" s="4" t="s">
         <v>0</v>
@@ -1517,7 +1512,7 @@
         <v>41647</v>
       </c>
       <c r="I8" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="J8" s="4"/>
       <c r="K8" s="4"/>
@@ -1526,7 +1521,7 @@
         <v>42012</v>
       </c>
       <c r="N8" s="4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="O8" s="4" t="s">
         <v>0</v>
@@ -1541,7 +1536,7 @@
         <v>41648</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E9" s="4" t="s">
         <v>1</v>
@@ -1554,7 +1549,7 @@
         <v>41647</v>
       </c>
       <c r="I9" s="4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="J9" s="4" t="s">
         <v>0</v>
@@ -1567,7 +1562,7 @@
         <v>42053</v>
       </c>
       <c r="N9" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="O9" s="4" t="s">
         <v>0</v>
@@ -1582,7 +1577,7 @@
         <v>41648</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E10" s="4" t="s">
         <v>1</v>
@@ -1595,7 +1590,7 @@
         <v>41647</v>
       </c>
       <c r="I10" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="J10" s="4" t="s">
         <v>0</v>
@@ -1608,7 +1603,7 @@
         <v>42053</v>
       </c>
       <c r="N10" s="4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="O10" s="4" t="s">
         <v>1</v>
@@ -1623,7 +1618,7 @@
         <v>41659</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E11" s="4" t="s">
         <v>1</v>
@@ -1636,7 +1631,7 @@
         <v>41647</v>
       </c>
       <c r="I11" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="J11" s="4"/>
       <c r="K11" s="4"/>
@@ -1645,7 +1640,7 @@
         <v>42074</v>
       </c>
       <c r="N11" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="O11" s="4" t="s">
         <v>0</v>
@@ -1660,10 +1655,10 @@
         <v>41659</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>0</v>
+        <v>41</v>
       </c>
       <c r="F12" s="4">
         <v>43</v>
@@ -1673,7 +1668,7 @@
         <v>41647</v>
       </c>
       <c r="I12" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="J12" s="4" t="s">
         <v>0</v>
@@ -1686,7 +1681,7 @@
         <v>42074</v>
       </c>
       <c r="N12" s="4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="O12" s="4" t="s">
         <v>1</v>
@@ -1701,10 +1696,10 @@
         <v>41659</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F13" s="4">
         <v>144</v>
@@ -1714,7 +1709,7 @@
         <v>41647</v>
       </c>
       <c r="I13" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="J13" s="4" t="s">
         <v>0</v>
@@ -1727,7 +1722,7 @@
         <v>42074</v>
       </c>
       <c r="N13" s="4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="O13" s="4" t="s">
         <v>0</v>
@@ -1742,10 +1737,10 @@
         <v>41711</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>1</v>
+        <v>41</v>
       </c>
       <c r="F14" s="4">
         <v>51</v>
@@ -1755,7 +1750,7 @@
         <v>41647</v>
       </c>
       <c r="I14" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="J14" s="4" t="s">
         <v>0</v>
@@ -1768,7 +1763,7 @@
         <v>42074</v>
       </c>
       <c r="N14" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="O14" s="4" t="s">
         <v>0</v>
@@ -1783,10 +1778,10 @@
         <v>41711</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F15" s="4">
         <v>44</v>
@@ -1796,7 +1791,7 @@
         <v>41647</v>
       </c>
       <c r="I15" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="J15" s="4" t="s">
         <v>0</v>
@@ -1809,12 +1804,14 @@
         <v>42102</v>
       </c>
       <c r="N15" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="O15" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="P15" s="4"/>
+      <c r="P15" s="4">
+        <v>0</v>
+      </c>
       <c r="Q15" s="5"/>
     </row>
     <row r="16" spans="3:17" ht="30" x14ac:dyDescent="0.3">
@@ -1822,10 +1819,10 @@
         <v>41711</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F16" s="4">
         <v>146</v>
@@ -1835,7 +1832,7 @@
         <v>41647</v>
       </c>
       <c r="I16" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="J16" s="4" t="s">
         <v>1</v>
@@ -1862,7 +1859,7 @@
         <v>41647</v>
       </c>
       <c r="I17" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="J17" s="4" t="s">
         <v>0</v>
@@ -1875,7 +1872,7 @@
         <v>42142</v>
       </c>
       <c r="N17" s="4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="O17" s="4" t="s">
         <v>1</v>
@@ -1895,7 +1892,7 @@
         <v>41647</v>
       </c>
       <c r="I18" s="4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="J18" s="4" t="s">
         <v>1</v>
@@ -1908,7 +1905,7 @@
         <v>42164</v>
       </c>
       <c r="N18" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="O18" s="4" t="s">
         <v>1</v>
@@ -1928,7 +1925,7 @@
         <v>41647</v>
       </c>
       <c r="I19" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="J19" s="4" t="s">
         <v>1</v>
@@ -1941,7 +1938,7 @@
         <v>42193</v>
       </c>
       <c r="N19" s="4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="O19" s="4" t="s">
         <v>1</v>
@@ -1961,7 +1958,7 @@
         <v>41647</v>
       </c>
       <c r="I20" s="4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="J20" s="4" t="s">
         <v>0</v>
@@ -1974,7 +1971,7 @@
         <v>42193</v>
       </c>
       <c r="N20" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="O20" s="4" t="s">
         <v>0</v>
@@ -1994,7 +1991,7 @@
         <v>41647</v>
       </c>
       <c r="I21" s="4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="J21" s="4"/>
       <c r="K21" s="4"/>
@@ -2015,7 +2012,7 @@
         <v>41647</v>
       </c>
       <c r="I22" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="J22" s="4" t="s">
         <v>0</v>
@@ -2040,7 +2037,7 @@
         <v>41647</v>
       </c>
       <c r="I23" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="J23" s="4"/>
       <c r="K23" s="4"/>
@@ -2061,7 +2058,7 @@
         <v>41688</v>
       </c>
       <c r="I24" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="J24" s="4" t="s">
         <v>0</v>
@@ -2086,7 +2083,7 @@
         <v>41688</v>
       </c>
       <c r="I25" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="J25" s="4" t="s">
         <v>1</v>
@@ -2111,7 +2108,7 @@
         <v>41688</v>
       </c>
       <c r="I26" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="J26" s="4" t="s">
         <v>0</v>
@@ -2196,7 +2193,7 @@
     </row>
     <row r="31" spans="3:17" ht="31" x14ac:dyDescent="0.35">
       <c r="C31" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D31" s="4"/>
       <c r="E31" s="4"/>
@@ -2204,7 +2201,7 @@
       <c r="G31" s="5"/>
       <c r="H31" s="8"/>
       <c r="I31" s="9" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="J31" s="5"/>
       <c r="K31" s="5"/>
@@ -2220,10 +2217,10 @@
         <v>5</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F32" s="5"/>
       <c r="G32" s="5"/>
@@ -2243,7 +2240,7 @@
         <v>28498</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E33" s="4">
         <v>37</v>
@@ -2266,7 +2263,7 @@
         <v>28498</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E34" s="4">
         <v>128</v>
@@ -2289,7 +2286,7 @@
         <v>28498</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E35" s="4">
         <v>42</v>
@@ -2312,7 +2309,7 @@
         <v>28498</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="E36" s="4">
         <v>37</v>
@@ -2335,7 +2332,7 @@
         <v>28498</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E37" s="4"/>
       <c r="F37" s="5"/>
@@ -2356,7 +2353,7 @@
         <v>28498</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E38" s="4">
         <v>48</v>
@@ -2379,7 +2376,7 @@
         <v>28498</v>
       </c>
       <c r="D39" s="4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E39" s="4">
         <v>45</v>
@@ -2402,7 +2399,7 @@
         <v>28498</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E40" s="4">
         <v>42</v>
@@ -2425,7 +2422,7 @@
         <v>28498</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E41" s="4">
         <v>52</v>
@@ -2448,7 +2445,7 @@
         <v>28498</v>
       </c>
       <c r="D42" s="4" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E42" s="4">
         <v>35</v>
@@ -2558,223 +2555,4 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H15"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="30" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="18.5" customWidth="1"/>
-    <col min="2" max="2" width="13.5" customWidth="1"/>
-    <col min="4" max="4" width="17.83203125" customWidth="1"/>
-    <col min="5" max="5" width="10.83203125" style="11"/>
-    <col min="6" max="8" width="10.83203125" style="5"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="23" t="s">
-        <v>7</v>
-      </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="23" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="23" t="s">
-        <v>23</v>
-      </c>
-      <c r="C2" s="23" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" s="23" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="24">
-        <v>42012</v>
-      </c>
-      <c r="B3" s="23" t="s">
-        <v>24</v>
-      </c>
-      <c r="C3" s="23" t="s">
-        <v>0</v>
-      </c>
-      <c r="D3" s="23">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="24">
-        <v>42053</v>
-      </c>
-      <c r="B4" s="23" t="s">
-        <v>24</v>
-      </c>
-      <c r="C4" s="23" t="s">
-        <v>0</v>
-      </c>
-      <c r="D4" s="23">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="24">
-        <v>42054</v>
-      </c>
-      <c r="B5" s="23" t="s">
-        <v>24</v>
-      </c>
-      <c r="C5" s="23" t="s">
-        <v>1</v>
-      </c>
-      <c r="D5" s="23">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="24">
-        <v>42074</v>
-      </c>
-      <c r="B6" s="23" t="s">
-        <v>31</v>
-      </c>
-      <c r="C6" s="23" t="s">
-        <v>0</v>
-      </c>
-      <c r="D6" s="23">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="24">
-        <v>42074</v>
-      </c>
-      <c r="B7" s="23" t="s">
-        <v>24</v>
-      </c>
-      <c r="C7" s="23" t="s">
-        <v>1</v>
-      </c>
-      <c r="D7" s="23">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="24">
-        <v>42074</v>
-      </c>
-      <c r="B8" s="23" t="s">
-        <v>31</v>
-      </c>
-      <c r="C8" s="23" t="s">
-        <v>0</v>
-      </c>
-      <c r="D8" s="23">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="24">
-        <v>42074</v>
-      </c>
-      <c r="B9" s="23" t="s">
-        <v>24</v>
-      </c>
-      <c r="C9" s="23" t="s">
-        <v>0</v>
-      </c>
-      <c r="D9" s="23">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="24">
-        <v>42102</v>
-      </c>
-      <c r="B10" s="23" t="s">
-        <v>31</v>
-      </c>
-      <c r="C10" s="23" t="s">
-        <v>1</v>
-      </c>
-      <c r="D10" s="23"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="24">
-        <v>42130</v>
-      </c>
-      <c r="B11" s="23"/>
-      <c r="C11" s="23"/>
-      <c r="D11" s="23"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" s="24">
-        <v>42142</v>
-      </c>
-      <c r="B12" s="23" t="s">
-        <v>24</v>
-      </c>
-      <c r="C12" s="23" t="s">
-        <v>1</v>
-      </c>
-      <c r="D12" s="23">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" s="24">
-        <v>42164</v>
-      </c>
-      <c r="B13" s="23" t="s">
-        <v>31</v>
-      </c>
-      <c r="C13" s="23" t="s">
-        <v>1</v>
-      </c>
-      <c r="D13" s="23">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" s="24">
-        <v>42193</v>
-      </c>
-      <c r="B14" s="23" t="s">
-        <v>31</v>
-      </c>
-      <c r="C14" s="23" t="s">
-        <v>1</v>
-      </c>
-      <c r="D14" s="23">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" s="24">
-        <v>42193</v>
-      </c>
-      <c r="B15" s="23" t="s">
-        <v>31</v>
-      </c>
-      <c r="C15" s="23" t="s">
-        <v>0</v>
-      </c>
-      <c r="D15" s="23">
-        <v>190</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter alignWithMargins="0"/>
-</worksheet>
 </file>
</xml_diff>